<commit_message>
atualização do ficheiro excel com a metrica Martin ....
</commit_message>
<xml_diff>
--- a/Phase 1/Sprint1/team_member_60441/data_collected_metrics.xlsx
+++ b/Phase 1/Sprint1/team_member_60441/data_collected_metrics.xlsx
@@ -5,24 +5,24 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1 - MartinPackagingMetric" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet 1 - Martin Packaging metr" sheetId="1" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="145">
-  <si>
-    <t>MartinPackagingMetrics</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="66">
+  <si>
+    <t>Martin Packaging metric</t>
   </si>
   <si>
     <t>Martin packaging metrics</t>
   </si>
   <si>
-    <t>Tue</t>
-  </si>
-  <si>
-    <t>29 Nov 2022 21:42:41 WET</t>
+    <t>quarta</t>
+  </si>
+  <si>
+    <t>30 nov. 2022 10:59:17 WET</t>
   </si>
   <si>
     <t>Package</t>
@@ -43,210 +43,75 @@
     <t>I</t>
   </si>
   <si>
-    <t>biz.ganttproject.impex.csv</t>
-  </si>
-  <si>
-    <t>0.18</t>
-  </si>
-  <si>
-    <t>0.17</t>
-  </si>
-  <si>
-    <t>0.99</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject</t>
   </si>
   <si>
-    <t>0.24</t>
-  </si>
-  <si>
-    <t>0.57</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.action</t>
   </si>
   <si>
-    <t>0.33</t>
-  </si>
-  <si>
-    <t>0.46</t>
-  </si>
-  <si>
-    <t>0.22</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.action.edit</t>
   </si>
   <si>
-    <t>0.00</t>
-  </si>
-  <si>
-    <t>0.08</t>
-  </si>
-  <si>
-    <t>0.92</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.action.help</t>
   </si>
   <si>
-    <t>0.04</t>
-  </si>
-  <si>
-    <t>0.70</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.action.project</t>
   </si>
   <si>
-    <t>0.07</t>
-  </si>
-  <si>
-    <t>0.03</t>
-  </si>
-  <si>
-    <t>0.97</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.action.resource</t>
   </si>
   <si>
-    <t>0.10</t>
-  </si>
-  <si>
-    <t>0.87</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.action.scroll</t>
   </si>
   <si>
-    <t>0.09</t>
-  </si>
-  <si>
-    <t>0.91</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.action.task</t>
   </si>
   <si>
-    <t>0.20</t>
-  </si>
-  <si>
-    <t>0.14</t>
-  </si>
-  <si>
-    <t>0.94</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.action.view</t>
   </si>
   <si>
-    <t>0.11</t>
-  </si>
-  <si>
-    <t>0.88</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.action.zoom</t>
   </si>
   <si>
-    <t>0.36</t>
-  </si>
-  <si>
-    <t>0.64</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.application</t>
   </si>
   <si>
-    <t>1.00</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.calendar</t>
   </si>
   <si>
-    <t>0.12</t>
-  </si>
-  <si>
-    <t>0.93</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.chart</t>
   </si>
   <si>
-    <t>0.34</t>
-  </si>
-  <si>
-    <t>0.71</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.chart.export</t>
   </si>
   <si>
-    <t>0.25</t>
-  </si>
-  <si>
-    <t>0.16</t>
-  </si>
-  <si>
-    <t>0.59</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.chart.gantt</t>
   </si>
   <si>
     <t>net.sourceforge.ganttproject.chart.item</t>
   </si>
   <si>
-    <t>0.90</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.chart.mouse</t>
   </si>
   <si>
-    <t>0.38</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.chart.overview</t>
   </si>
   <si>
-    <t>0.47</t>
-  </si>
-  <si>
-    <t>0.52</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.client</t>
   </si>
   <si>
     <t>net.sourceforge.ganttproject.document</t>
   </si>
   <si>
-    <t>0.37</t>
-  </si>
-  <si>
-    <t>0.06</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.document.webdav</t>
   </si>
   <si>
-    <t>0.95</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.excel</t>
   </si>
   <si>
-    <t>0.75</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.export</t>
   </si>
   <si>
-    <t>0.83</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.filter</t>
   </si>
   <si>
@@ -256,79 +121,37 @@
     <t>net.sourceforge.ganttproject.gui</t>
   </si>
   <si>
-    <t>0.27</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.gui.about</t>
   </si>
   <si>
     <t>net.sourceforge.ganttproject.gui.options</t>
   </si>
   <si>
-    <t>0.80</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.gui.options.model</t>
   </si>
   <si>
     <t>net.sourceforge.ganttproject.gui.projectwizard</t>
   </si>
   <si>
-    <t>0.15</t>
-  </si>
-  <si>
-    <t>0.86</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.gui.scrolling</t>
   </si>
   <si>
-    <t>0.67</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.gui.tableView</t>
   </si>
   <si>
-    <t>0.02</t>
-  </si>
-  <si>
-    <t>0.96</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.gui.taskproperties</t>
   </si>
   <si>
     <t>net.sourceforge.ganttproject.gui.view</t>
   </si>
   <si>
-    <t>0.50</t>
-  </si>
-  <si>
-    <t>0.01</t>
-  </si>
-  <si>
-    <t>0.51</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.gui.window</t>
   </si>
   <si>
-    <t>0.40</t>
-  </si>
-  <si>
-    <t>0.56</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.gui.zoom</t>
   </si>
   <si>
-    <t>0.61</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.importer</t>
-  </si>
-  <si>
-    <t>0.82</t>
   </si>
   <si>
     <r>
@@ -343,60 +166,27 @@
     </r>
   </si>
   <si>
-    <t>0.29</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.language</t>
   </si>
   <si>
-    <t>0.68</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.parser</t>
   </si>
   <si>
-    <t>0.13</t>
-  </si>
-  <si>
-    <t>0.66</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.plugins</t>
   </si>
   <si>
-    <t>0.72</t>
-  </si>
-  <si>
-    <t>0.28</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.print</t>
   </si>
   <si>
     <t>net.sourceforge.ganttproject.resource</t>
   </si>
   <si>
-    <t>0.35</t>
-  </si>
-  <si>
-    <t>0.44</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.roles</t>
   </si>
   <si>
-    <t>0.48</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.search</t>
   </si>
   <si>
-    <t>0.23</t>
-  </si>
-  <si>
-    <t>0.89</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.shape</t>
   </si>
   <si>
@@ -406,21 +196,9 @@
     <t>net.sourceforge.ganttproject.task.algorithm</t>
   </si>
   <si>
-    <t>0.31</t>
-  </si>
-  <si>
-    <t>0.58</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.task.dependency</t>
   </si>
   <si>
-    <t>0.42</t>
-  </si>
-  <si>
-    <t>0.45</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.task.dependency.constraint</t>
   </si>
   <si>
@@ -430,31 +208,16 @@
     <t>net.sourceforge.ganttproject.task.hierarchy</t>
   </si>
   <si>
-    <t>0.79</t>
-  </si>
-  <si>
-    <t>0.21</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.undo</t>
   </si>
   <si>
-    <t>0.43</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.util</t>
   </si>
   <si>
-    <t>0.73</t>
-  </si>
-  <si>
     <t>net.sourceforge.ganttproject.util.collect</t>
   </si>
   <si>
     <t>net.sourceforge.ganttproject.wizard</t>
-  </si>
-  <si>
-    <t>org.ganttproject</t>
   </si>
 </sst>
 </file>
@@ -628,7 +391,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -656,13 +419,10 @@
     <xf numFmtId="49" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1747,16 +1507,16 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:F61"/>
+  <dimension ref="A2:F59"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.33333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="46.6719" style="1" customWidth="1"/>
-    <col min="2" max="2" width="4.85156" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.1719" style="1" customWidth="1"/>
-    <col min="4" max="4" width="5.67188" style="1" customWidth="1"/>
+    <col min="2" max="2" width="6.67188" style="1" customWidth="1"/>
+    <col min="3" max="3" width="22.3516" style="1" customWidth="1"/>
+    <col min="4" max="4" width="3.5" style="1" customWidth="1"/>
     <col min="5" max="6" width="4.67188" style="1" customWidth="1"/>
     <col min="7" max="16384" width="8.35156" style="1" customWidth="1"/>
   </cols>
@@ -1809,1160 +1569,1120 @@
       <c r="A4" t="s" s="8">
         <v>10</v>
       </c>
-      <c r="B4" t="s" s="9">
-        <v>11</v>
+      <c r="B4" s="9">
+        <v>0.17</v>
       </c>
       <c r="C4" s="10">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D4" s="10">
-        <v>431</v>
-      </c>
-      <c r="E4" t="s" s="11">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s" s="11">
-        <v>13</v>
+        <v>0</v>
+      </c>
+      <c r="E4" s="10">
+        <v>0.83</v>
+      </c>
+      <c r="F4" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="5" ht="20.05" customHeight="1">
       <c r="A5" t="s" s="8">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s" s="9">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B5" s="9">
+        <v>0.33</v>
       </c>
       <c r="C5" s="10">
-        <v>1.875</v>
+        <v>0</v>
       </c>
       <c r="D5" s="10">
-        <v>2.733</v>
-      </c>
-      <c r="E5" t="s" s="11">
-        <v>15</v>
-      </c>
-      <c r="F5" t="s" s="11">
-        <v>16</v>
+        <v>0</v>
+      </c>
+      <c r="E5" s="10">
+        <v>0.67</v>
+      </c>
+      <c r="F5" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="6" ht="20.05" customHeight="1">
       <c r="A6" t="s" s="8">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s" s="9">
-        <v>18</v>
+        <v>12</v>
+      </c>
+      <c r="B6" s="9">
+        <v>0</v>
       </c>
       <c r="C6" s="10">
-        <v>481</v>
+        <v>0</v>
       </c>
       <c r="D6" s="10">
-        <v>123</v>
-      </c>
-      <c r="E6" t="s" s="11">
-        <v>19</v>
-      </c>
-      <c r="F6" t="s" s="11">
-        <v>20</v>
+        <v>0</v>
+      </c>
+      <c r="E6" s="10">
+        <v>1</v>
+      </c>
+      <c r="F6" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="7" ht="20.05" customHeight="1">
       <c r="A7" t="s" s="8">
-        <v>21</v>
-      </c>
-      <c r="B7" t="s" s="9">
-        <v>22</v>
+        <v>13</v>
+      </c>
+      <c r="B7" s="9">
+        <v>0</v>
       </c>
       <c r="C7" s="10">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="D7" s="10">
-        <v>158</v>
-      </c>
-      <c r="E7" t="s" s="11">
-        <v>23</v>
-      </c>
-      <c r="F7" t="s" s="11">
-        <v>24</v>
+        <v>0</v>
+      </c>
+      <c r="E7" s="10">
+        <v>1</v>
+      </c>
+      <c r="F7" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="8" ht="20.05" customHeight="1">
       <c r="A8" t="s" s="8">
-        <v>25</v>
-      </c>
-      <c r="B8" t="s" s="9">
-        <v>22</v>
+        <v>14</v>
+      </c>
+      <c r="B8" s="9">
+        <v>0.07000000000000001</v>
       </c>
       <c r="C8" s="10">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D8" s="10">
-        <v>71</v>
-      </c>
-      <c r="E8" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="F8" t="s" s="11">
-        <v>27</v>
+        <v>0</v>
+      </c>
+      <c r="E8" s="10">
+        <v>0.93</v>
+      </c>
+      <c r="F8" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="9" ht="20.05" customHeight="1">
       <c r="A9" t="s" s="8">
-        <v>28</v>
-      </c>
-      <c r="B9" t="s" s="9">
-        <v>29</v>
+        <v>15</v>
+      </c>
+      <c r="B9" s="9">
+        <v>0.1</v>
       </c>
       <c r="C9" s="10">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D9" s="10">
-        <v>208</v>
-      </c>
-      <c r="E9" t="s" s="11">
-        <v>30</v>
-      </c>
-      <c r="F9" t="s" s="11">
-        <v>31</v>
+        <v>0</v>
+      </c>
+      <c r="E9" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="F9" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="10" ht="20.05" customHeight="1">
       <c r="A10" t="s" s="8">
-        <v>32</v>
-      </c>
-      <c r="B10" t="s" s="9">
-        <v>33</v>
+        <v>16</v>
+      </c>
+      <c r="B10" s="9">
+        <v>0</v>
       </c>
       <c r="C10" s="10">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="D10" s="10">
-        <v>206</v>
-      </c>
-      <c r="E10" t="s" s="11">
-        <v>30</v>
-      </c>
-      <c r="F10" t="s" s="11">
-        <v>34</v>
+        <v>0</v>
+      </c>
+      <c r="E10" s="10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="11" ht="20.05" customHeight="1">
       <c r="A11" t="s" s="8">
-        <v>35</v>
-      </c>
-      <c r="B11" t="s" s="9">
-        <v>22</v>
+        <v>17</v>
+      </c>
+      <c r="B11" s="9">
+        <v>0.2</v>
       </c>
       <c r="C11" s="10">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D11" s="10">
-        <v>62</v>
-      </c>
-      <c r="E11" t="s" s="11">
-        <v>36</v>
-      </c>
-      <c r="F11" t="s" s="11">
-        <v>37</v>
+        <v>0</v>
+      </c>
+      <c r="E11" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="F11" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="12" ht="20.05" customHeight="1">
       <c r="A12" t="s" s="8">
-        <v>38</v>
-      </c>
-      <c r="B12" t="s" s="9">
-        <v>39</v>
+        <v>18</v>
+      </c>
+      <c r="B12" s="9">
+        <v>0</v>
       </c>
       <c r="C12" s="10">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="D12" s="10">
-        <v>404</v>
-      </c>
-      <c r="E12" t="s" s="11">
-        <v>40</v>
-      </c>
-      <c r="F12" t="s" s="11">
-        <v>41</v>
+        <v>0</v>
+      </c>
+      <c r="E12" s="10">
+        <v>1</v>
+      </c>
+      <c r="F12" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="13" ht="20.05" customHeight="1">
       <c r="A13" t="s" s="8">
-        <v>42</v>
-      </c>
-      <c r="B13" t="s" s="9">
-        <v>22</v>
+        <v>19</v>
+      </c>
+      <c r="B13" s="9">
+        <v>0</v>
       </c>
       <c r="C13" s="10">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D13" s="10">
-        <v>48</v>
-      </c>
-      <c r="E13" t="s" s="11">
-        <v>43</v>
-      </c>
-      <c r="F13" t="s" s="11">
-        <v>44</v>
+        <v>0</v>
+      </c>
+      <c r="E13" s="10">
+        <v>1</v>
+      </c>
+      <c r="F13" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="14" ht="20.05" customHeight="1">
       <c r="A14" t="s" s="8">
-        <v>45</v>
-      </c>
-      <c r="B14" t="s" s="9">
-        <v>22</v>
+        <v>20</v>
+      </c>
+      <c r="B14" s="9">
+        <v>0</v>
       </c>
       <c r="C14" s="10">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D14" s="10">
-        <v>21</v>
-      </c>
-      <c r="E14" t="s" s="11">
-        <v>46</v>
-      </c>
-      <c r="F14" t="s" s="11">
-        <v>47</v>
+        <v>0</v>
+      </c>
+      <c r="E14" s="10">
+        <v>1</v>
+      </c>
+      <c r="F14" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="15" ht="20.05" customHeight="1">
       <c r="A15" t="s" s="8">
-        <v>48</v>
-      </c>
-      <c r="B15" t="s" s="9">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="B15" s="9">
+        <v>0.12</v>
       </c>
       <c r="C15" s="10">
         <v>0</v>
       </c>
       <c r="D15" s="10">
-        <v>12</v>
-      </c>
-      <c r="E15" t="s" s="11">
-        <v>22</v>
-      </c>
-      <c r="F15" t="s" s="11">
-        <v>49</v>
+        <v>0</v>
+      </c>
+      <c r="E15" s="10">
+        <v>0.88</v>
+      </c>
+      <c r="F15" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="16" ht="20.05" customHeight="1">
       <c r="A16" t="s" s="8">
-        <v>50</v>
-      </c>
-      <c r="B16" t="s" s="9">
-        <v>51</v>
+        <v>22</v>
+      </c>
+      <c r="B16" s="9">
+        <v>0.34</v>
       </c>
       <c r="C16" s="10">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D16" s="10">
-        <v>225</v>
-      </c>
-      <c r="E16" t="s" s="11">
-        <v>23</v>
-      </c>
-      <c r="F16" t="s" s="11">
-        <v>52</v>
+        <v>0</v>
+      </c>
+      <c r="E16" s="10">
+        <v>0.66</v>
+      </c>
+      <c r="F16" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="17" ht="20.05" customHeight="1">
       <c r="A17" t="s" s="8">
-        <v>53</v>
-      </c>
-      <c r="B17" t="s" s="9">
-        <v>54</v>
+        <v>23</v>
+      </c>
+      <c r="B17" s="9">
+        <v>0.25</v>
       </c>
       <c r="C17" s="10">
-        <v>429</v>
+        <v>0</v>
       </c>
       <c r="D17" s="10">
-        <v>1.172</v>
-      </c>
-      <c r="E17" t="s" s="11">
-        <v>29</v>
-      </c>
-      <c r="F17" t="s" s="11">
-        <v>55</v>
+        <v>0</v>
+      </c>
+      <c r="E17" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="F17" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="18" ht="20.05" customHeight="1">
       <c r="A18" t="s" s="8">
-        <v>56</v>
-      </c>
-      <c r="B18" t="s" s="9">
-        <v>57</v>
+        <v>24</v>
+      </c>
+      <c r="B18" s="9">
+        <v>0</v>
       </c>
       <c r="C18" s="10">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="D18" s="10">
-        <v>78</v>
-      </c>
-      <c r="E18" t="s" s="11">
-        <v>58</v>
-      </c>
-      <c r="F18" t="s" s="11">
-        <v>59</v>
+        <v>0</v>
+      </c>
+      <c r="E18" s="10">
+        <v>1</v>
+      </c>
+      <c r="F18" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="19" ht="20.05" customHeight="1">
       <c r="A19" t="s" s="8">
-        <v>60</v>
-      </c>
-      <c r="B19" t="s" s="9">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="B19" s="9">
+        <v>0</v>
       </c>
       <c r="C19" s="10">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="D19" s="10">
-        <v>471</v>
-      </c>
-      <c r="E19" t="s" s="11">
-        <v>29</v>
-      </c>
-      <c r="F19" t="s" s="11">
-        <v>52</v>
+        <v>0</v>
+      </c>
+      <c r="E19" s="10">
+        <v>1</v>
+      </c>
+      <c r="F19" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="20" ht="20.05" customHeight="1">
       <c r="A20" t="s" s="8">
-        <v>61</v>
-      </c>
-      <c r="B20" t="s" s="9">
-        <v>22</v>
+        <v>26</v>
+      </c>
+      <c r="B20" s="9">
+        <v>0.38</v>
       </c>
       <c r="C20" s="10">
-        <v>71</v>
+        <v>0</v>
       </c>
       <c r="D20" s="10">
-        <v>8</v>
-      </c>
-      <c r="E20" t="s" s="11">
-        <v>62</v>
-      </c>
-      <c r="F20" t="s" s="11">
-        <v>33</v>
+        <v>0</v>
+      </c>
+      <c r="E20" s="10">
+        <v>0.62</v>
+      </c>
+      <c r="F20" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="21" ht="20.05" customHeight="1">
       <c r="A21" t="s" s="8">
-        <v>63</v>
-      </c>
-      <c r="B21" t="s" s="9">
-        <v>64</v>
+        <v>27</v>
+      </c>
+      <c r="B21" s="9">
+        <v>0</v>
       </c>
       <c r="C21" s="10">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="D21" s="10">
-        <v>250</v>
-      </c>
-      <c r="E21" t="s" s="11">
-        <v>57</v>
-      </c>
-      <c r="F21" t="s" s="11">
-        <v>34</v>
+        <v>0</v>
+      </c>
+      <c r="E21" s="10">
+        <v>1</v>
+      </c>
+      <c r="F21" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="22" ht="20.05" customHeight="1">
       <c r="A22" t="s" s="8">
-        <v>65</v>
-      </c>
-      <c r="B22" t="s" s="9">
-        <v>22</v>
+        <v>28</v>
+      </c>
+      <c r="B22" s="9">
+        <v>0</v>
       </c>
       <c r="C22" s="10">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="D22" s="10">
-        <v>87</v>
-      </c>
-      <c r="E22" t="s" s="11">
-        <v>66</v>
-      </c>
-      <c r="F22" t="s" s="11">
-        <v>67</v>
+        <v>0</v>
+      </c>
+      <c r="E22" s="10">
+        <v>1</v>
+      </c>
+      <c r="F22" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="23" ht="20.05" customHeight="1">
       <c r="A23" t="s" s="8">
-        <v>68</v>
-      </c>
-      <c r="B23" t="s" s="9">
-        <v>22</v>
+        <v>29</v>
+      </c>
+      <c r="B23" s="9">
+        <v>0.37</v>
       </c>
       <c r="C23" s="10">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D23" s="10">
-        <v>91</v>
-      </c>
-      <c r="E23" t="s" s="11">
-        <v>29</v>
-      </c>
-      <c r="F23" t="s" s="11">
-        <v>52</v>
+        <v>0</v>
+      </c>
+      <c r="E23" s="10">
+        <v>0.63</v>
+      </c>
+      <c r="F23" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="24" ht="20.05" customHeight="1">
       <c r="A24" t="s" s="8">
-        <v>69</v>
-      </c>
-      <c r="B24" t="s" s="9">
-        <v>70</v>
+        <v>30</v>
+      </c>
+      <c r="B24" s="9">
+        <v>0.11</v>
       </c>
       <c r="C24" s="10">
-        <v>220</v>
+        <v>0</v>
       </c>
       <c r="D24" s="10">
-        <v>296</v>
-      </c>
-      <c r="E24" t="s" s="11">
-        <v>71</v>
-      </c>
-      <c r="F24" t="s" s="11">
-        <v>67</v>
+        <v>0</v>
+      </c>
+      <c r="E24" s="10">
+        <v>0.89</v>
+      </c>
+      <c r="F24" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="25" ht="20.05" customHeight="1">
       <c r="A25" t="s" s="8">
-        <v>72</v>
-      </c>
-      <c r="B25" t="s" s="9">
-        <v>43</v>
+        <v>31</v>
+      </c>
+      <c r="B25" s="9">
+        <v>0</v>
       </c>
       <c r="C25" s="10">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D25" s="10">
-        <v>322</v>
-      </c>
-      <c r="E25" t="s" s="11">
-        <v>71</v>
-      </c>
-      <c r="F25" t="s" s="11">
-        <v>73</v>
+        <v>0</v>
+      </c>
+      <c r="E25" s="10">
+        <v>1</v>
+      </c>
+      <c r="F25" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="26" ht="20.05" customHeight="1">
       <c r="A26" t="s" s="8">
-        <v>74</v>
-      </c>
-      <c r="B26" t="s" s="9">
-        <v>22</v>
+        <v>32</v>
+      </c>
+      <c r="B26" s="9">
+        <v>0.25</v>
       </c>
       <c r="C26" s="10">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D26" s="10">
-        <v>9</v>
-      </c>
-      <c r="E26" t="s" s="11">
-        <v>57</v>
-      </c>
-      <c r="F26" t="s" s="11">
-        <v>75</v>
+        <v>0</v>
+      </c>
+      <c r="E26" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="F26" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="27" ht="20.05" customHeight="1">
       <c r="A27" t="s" s="8">
-        <v>76</v>
-      </c>
-      <c r="B27" t="s" s="9">
-        <v>57</v>
+        <v>33</v>
+      </c>
+      <c r="B27" s="9">
+        <v>0</v>
       </c>
       <c r="C27" s="10">
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="D27" s="10">
-        <v>305</v>
-      </c>
-      <c r="E27" t="s" s="11">
-        <v>30</v>
-      </c>
-      <c r="F27" t="s" s="11">
-        <v>77</v>
+        <v>0</v>
+      </c>
+      <c r="E27" s="10">
+        <v>1</v>
+      </c>
+      <c r="F27" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="28" ht="20.05" customHeight="1">
       <c r="A28" t="s" s="8">
-        <v>78</v>
-      </c>
-      <c r="B28" t="s" s="9">
-        <v>22</v>
+        <v>34</v>
+      </c>
+      <c r="B28" s="9">
+        <v>0</v>
       </c>
       <c r="C28" s="10">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D28" s="10">
         <v>0</v>
       </c>
-      <c r="E28" t="s" s="11">
-        <v>49</v>
-      </c>
-      <c r="F28" t="s" s="11">
-        <v>22</v>
+      <c r="E28" s="10">
+        <v>1</v>
+      </c>
+      <c r="F28" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="29" ht="20.05" customHeight="1">
       <c r="A29" t="s" s="8">
-        <v>79</v>
-      </c>
-      <c r="B29" t="s" s="9">
-        <v>22</v>
+        <v>35</v>
+      </c>
+      <c r="B29" s="9">
+        <v>0.27</v>
       </c>
       <c r="C29" s="10">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="D29" s="10">
         <v>0</v>
       </c>
-      <c r="E29" t="s" s="11">
-        <v>49</v>
-      </c>
-      <c r="F29" t="s" s="11">
-        <v>22</v>
+      <c r="E29" s="10">
+        <v>0.73</v>
+      </c>
+      <c r="F29" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="30" ht="20.05" customHeight="1">
       <c r="A30" t="s" s="8">
-        <v>80</v>
-      </c>
-      <c r="B30" t="s" s="9">
-        <v>81</v>
+        <v>36</v>
+      </c>
+      <c r="B30" s="9">
+        <v>0</v>
       </c>
       <c r="C30" s="10">
-        <v>1.295</v>
+        <v>0</v>
       </c>
       <c r="D30" s="10">
-        <v>851</v>
-      </c>
-      <c r="E30" t="s" s="11">
-        <v>18</v>
-      </c>
-      <c r="F30" t="s" s="11">
-        <v>64</v>
+        <v>0</v>
+      </c>
+      <c r="E30" s="10">
+        <v>1</v>
+      </c>
+      <c r="F30" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="31" ht="20.05" customHeight="1">
       <c r="A31" t="s" s="8">
-        <v>82</v>
-      </c>
-      <c r="B31" t="s" s="9">
-        <v>22</v>
+        <v>37</v>
+      </c>
+      <c r="B31" s="9">
+        <v>0.22</v>
       </c>
       <c r="C31" s="10">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D31" s="10">
-        <v>42</v>
-      </c>
-      <c r="E31" t="s" s="11">
-        <v>51</v>
-      </c>
-      <c r="F31" t="s" s="11">
-        <v>44</v>
+        <v>0</v>
+      </c>
+      <c r="E31" s="10">
+        <v>0.78</v>
+      </c>
+      <c r="F31" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="32" ht="20.05" customHeight="1">
       <c r="A32" t="s" s="8">
-        <v>83</v>
-      </c>
-      <c r="B32" t="s" s="9">
-        <v>20</v>
+        <v>38</v>
+      </c>
+      <c r="B32" s="9">
+        <v>1</v>
       </c>
       <c r="C32" s="10">
-        <v>214</v>
+        <v>0</v>
       </c>
       <c r="D32" s="10">
-        <v>646</v>
-      </c>
-      <c r="E32" t="s" s="11">
-        <v>30</v>
-      </c>
-      <c r="F32" t="s" s="11">
-        <v>84</v>
+        <v>0</v>
+      </c>
+      <c r="E32" s="10">
+        <v>0</v>
+      </c>
+      <c r="F32" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="33" ht="20.05" customHeight="1">
       <c r="A33" t="s" s="8">
-        <v>85</v>
-      </c>
-      <c r="B33" t="s" s="9">
-        <v>49</v>
+        <v>39</v>
+      </c>
+      <c r="B33" s="9">
+        <v>0.15</v>
       </c>
       <c r="C33" s="10">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="D33" s="10">
-        <v>55</v>
-      </c>
-      <c r="E33" t="s" s="11">
-        <v>16</v>
-      </c>
-      <c r="F33" t="s" s="11">
-        <v>16</v>
+        <v>0</v>
+      </c>
+      <c r="E33" s="10">
+        <v>0.85</v>
+      </c>
+      <c r="F33" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="34" ht="20.05" customHeight="1">
       <c r="A34" t="s" s="8">
-        <v>86</v>
-      </c>
-      <c r="B34" t="s" s="9">
-        <v>87</v>
+        <v>40</v>
+      </c>
+      <c r="B34" s="9">
+        <v>0.67</v>
       </c>
       <c r="C34" s="10">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="D34" s="10">
-        <v>204</v>
-      </c>
-      <c r="E34" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="F34" t="s" s="11">
-        <v>88</v>
+        <v>0</v>
+      </c>
+      <c r="E34" s="10">
+        <v>0.33</v>
+      </c>
+      <c r="F34" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="35" ht="20.05" customHeight="1">
       <c r="A35" t="s" s="8">
-        <v>89</v>
-      </c>
-      <c r="B35" t="s" s="9">
-        <v>90</v>
+        <v>41</v>
+      </c>
+      <c r="B35" s="9">
+        <v>0</v>
       </c>
       <c r="C35" s="10">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="D35" s="10">
-        <v>3</v>
-      </c>
-      <c r="E35" t="s" s="11">
-        <v>58</v>
-      </c>
-      <c r="F35" t="s" s="11">
-        <v>11</v>
+        <v>0</v>
+      </c>
+      <c r="E35" s="10">
+        <v>1</v>
+      </c>
+      <c r="F35" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="36" ht="20.05" customHeight="1">
       <c r="A36" t="s" s="8">
-        <v>91</v>
-      </c>
-      <c r="B36" t="s" s="9">
-        <v>22</v>
+        <v>42</v>
+      </c>
+      <c r="B36" s="9">
+        <v>0.17</v>
       </c>
       <c r="C36" s="10">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D36" s="10">
-        <v>188</v>
-      </c>
-      <c r="E36" t="s" s="11">
-        <v>92</v>
-      </c>
-      <c r="F36" t="s" s="11">
-        <v>93</v>
+        <v>0</v>
+      </c>
+      <c r="E36" s="10">
+        <v>0.83</v>
+      </c>
+      <c r="F36" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="37" ht="20.05" customHeight="1">
       <c r="A37" t="s" s="8">
-        <v>94</v>
-      </c>
-      <c r="B37" t="s" s="9">
-        <v>12</v>
+        <v>43</v>
+      </c>
+      <c r="B37" s="9">
+        <v>0.5</v>
       </c>
       <c r="C37" s="10">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="D37" s="10">
-        <v>409</v>
-      </c>
-      <c r="E37" t="s" s="11">
-        <v>33</v>
-      </c>
-      <c r="F37" t="s" s="11">
-        <v>52</v>
+        <v>0</v>
+      </c>
+      <c r="E37" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="F37" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="38" ht="20.05" customHeight="1">
       <c r="A38" t="s" s="8">
-        <v>95</v>
-      </c>
-      <c r="B38" t="s" s="9">
-        <v>96</v>
+        <v>44</v>
+      </c>
+      <c r="B38" s="9">
+        <v>0</v>
       </c>
       <c r="C38" s="10">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="D38" s="10">
-        <v>45</v>
-      </c>
-      <c r="E38" t="s" s="11">
-        <v>97</v>
-      </c>
-      <c r="F38" t="s" s="11">
-        <v>98</v>
+        <v>0</v>
+      </c>
+      <c r="E38" s="10">
+        <v>1</v>
+      </c>
+      <c r="F38" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="39" ht="20.05" customHeight="1">
       <c r="A39" t="s" s="8">
-        <v>99</v>
-      </c>
-      <c r="B39" t="s" s="9">
-        <v>22</v>
+        <v>45</v>
+      </c>
+      <c r="B39" s="9">
+        <v>0.25</v>
       </c>
       <c r="C39" s="10">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D39" s="10">
-        <v>6</v>
-      </c>
-      <c r="E39" t="s" s="11">
-        <v>100</v>
-      </c>
-      <c r="F39" t="s" s="11">
-        <v>101</v>
+        <v>0</v>
+      </c>
+      <c r="E39" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="F39" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="40" ht="20.05" customHeight="1">
       <c r="A40" t="s" s="8">
-        <v>102</v>
-      </c>
-      <c r="B40" t="s" s="9">
-        <v>57</v>
+        <v>46</v>
+      </c>
+      <c r="B40" s="9">
+        <v>0.27</v>
       </c>
       <c r="C40" s="10">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="D40" s="10">
-        <v>10</v>
-      </c>
-      <c r="E40" t="s" s="11">
-        <v>103</v>
-      </c>
-      <c r="F40" t="s" s="11">
-        <v>71</v>
+        <v>0</v>
+      </c>
+      <c r="E40" s="10">
+        <v>0.73</v>
+      </c>
+      <c r="F40" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="41" ht="20.05" customHeight="1">
       <c r="A41" t="s" s="8">
-        <v>104</v>
-      </c>
-      <c r="B41" t="s" s="9">
-        <v>81</v>
+        <v>47</v>
+      </c>
+      <c r="B41" s="9">
+        <v>0.06</v>
       </c>
       <c r="C41" s="10">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="D41" s="10">
-        <v>244</v>
-      </c>
-      <c r="E41" t="s" s="11">
-        <v>36</v>
-      </c>
-      <c r="F41" t="s" s="11">
-        <v>105</v>
+        <v>0</v>
+      </c>
+      <c r="E41" s="10">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="F41" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="42" ht="20.05" customHeight="1">
       <c r="A42" t="s" s="8">
-        <v>106</v>
-      </c>
-      <c r="B42" t="s" s="9">
-        <v>71</v>
+        <v>48</v>
+      </c>
+      <c r="B42" s="9">
+        <v>0.29</v>
       </c>
       <c r="C42" s="10">
-        <v>242</v>
+        <v>0</v>
       </c>
       <c r="D42" s="10">
-        <v>460</v>
-      </c>
-      <c r="E42" t="s" s="11">
-        <v>107</v>
-      </c>
-      <c r="F42" t="s" s="11">
-        <v>47</v>
+        <v>0</v>
+      </c>
+      <c r="E42" s="10">
+        <v>0.71</v>
+      </c>
+      <c r="F42" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="43" ht="20.05" customHeight="1">
       <c r="A43" t="s" s="8">
-        <v>108</v>
-      </c>
-      <c r="B43" t="s" s="9">
-        <v>107</v>
+        <v>49</v>
+      </c>
+      <c r="B43" s="9">
+        <v>0.2</v>
       </c>
       <c r="C43" s="10">
-        <v>937</v>
+        <v>0</v>
       </c>
       <c r="D43" s="10">
-        <v>29</v>
-      </c>
-      <c r="E43" t="s" s="11">
-        <v>109</v>
-      </c>
-      <c r="F43" t="s" s="11">
-        <v>30</v>
+        <v>0</v>
+      </c>
+      <c r="E43" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="F43" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="44" ht="20.05" customHeight="1">
       <c r="A44" t="s" s="8">
-        <v>110</v>
-      </c>
-      <c r="B44" t="s" s="9">
-        <v>39</v>
+        <v>50</v>
+      </c>
+      <c r="B44" s="9">
+        <v>0</v>
       </c>
       <c r="C44" s="10">
-        <v>162</v>
+        <v>0</v>
       </c>
       <c r="D44" s="10">
-        <v>326</v>
-      </c>
-      <c r="E44" t="s" s="11">
-        <v>111</v>
-      </c>
-      <c r="F44" t="s" s="11">
-        <v>112</v>
+        <v>0</v>
+      </c>
+      <c r="E44" s="10">
+        <v>1</v>
+      </c>
+      <c r="F44" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="45" ht="20.05" customHeight="1">
       <c r="A45" t="s" s="8">
-        <v>113</v>
-      </c>
-      <c r="B45" t="s" s="9">
-        <v>22</v>
+        <v>51</v>
+      </c>
+      <c r="B45" s="9">
+        <v>0</v>
       </c>
       <c r="C45" s="10">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="D45" s="10">
-        <v>8</v>
-      </c>
-      <c r="E45" t="s" s="11">
-        <v>114</v>
-      </c>
-      <c r="F45" t="s" s="11">
-        <v>115</v>
+        <v>0</v>
+      </c>
+      <c r="E45" s="10">
+        <v>1</v>
+      </c>
+      <c r="F45" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="46" ht="20.05" customHeight="1">
       <c r="A46" t="s" s="8">
-        <v>116</v>
-      </c>
-      <c r="B46" t="s" s="9">
-        <v>22</v>
+        <v>52</v>
+      </c>
+      <c r="B46" s="9">
+        <v>0.35</v>
       </c>
       <c r="C46" s="10">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D46" s="10">
-        <v>94</v>
-      </c>
-      <c r="E46" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="F46" t="s" s="11">
-        <v>93</v>
+        <v>0</v>
+      </c>
+      <c r="E46" s="10">
+        <v>0.65</v>
+      </c>
+      <c r="F46" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="47" ht="20.05" customHeight="1">
       <c r="A47" t="s" s="8">
-        <v>117</v>
-      </c>
-      <c r="B47" t="s" s="9">
-        <v>118</v>
+        <v>53</v>
+      </c>
+      <c r="B47" s="9">
+        <v>0.4</v>
       </c>
       <c r="C47" s="10">
-        <v>669</v>
+        <v>0</v>
       </c>
       <c r="D47" s="10">
-        <v>170</v>
-      </c>
-      <c r="E47" t="s" s="11">
-        <v>119</v>
-      </c>
-      <c r="F47" t="s" s="11">
-        <v>39</v>
+        <v>0</v>
+      </c>
+      <c r="E47" s="10">
+        <v>0.6</v>
+      </c>
+      <c r="F47" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="48" ht="20.05" customHeight="1">
       <c r="A48" t="s" s="8">
-        <v>120</v>
-      </c>
-      <c r="B48" t="s" s="9">
-        <v>100</v>
+        <v>54</v>
+      </c>
+      <c r="B48" s="9">
+        <v>0.33</v>
       </c>
       <c r="C48" s="10">
-        <v>265</v>
+        <v>0</v>
       </c>
       <c r="D48" s="10">
-        <v>36</v>
-      </c>
-      <c r="E48" t="s" s="11">
-        <v>121</v>
-      </c>
-      <c r="F48" t="s" s="11">
-        <v>111</v>
+        <v>0</v>
+      </c>
+      <c r="E48" s="10">
+        <v>0.67</v>
+      </c>
+      <c r="F48" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="49" ht="20.05" customHeight="1">
       <c r="A49" t="s" s="8">
-        <v>122</v>
-      </c>
-      <c r="B49" t="s" s="9">
-        <v>18</v>
+        <v>55</v>
+      </c>
+      <c r="B49" s="9">
+        <v>0</v>
       </c>
       <c r="C49" s="10">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D49" s="10">
-        <v>69</v>
-      </c>
-      <c r="E49" t="s" s="11">
-        <v>123</v>
-      </c>
-      <c r="F49" t="s" s="11">
-        <v>124</v>
+        <v>0</v>
+      </c>
+      <c r="E49" s="10">
+        <v>1</v>
+      </c>
+      <c r="F49" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="50" ht="20.05" customHeight="1">
       <c r="A50" t="s" s="8">
-        <v>125</v>
-      </c>
-      <c r="B50" t="s" s="9">
-        <v>22</v>
+        <v>56</v>
+      </c>
+      <c r="B50" s="9">
+        <v>0.33</v>
       </c>
       <c r="C50" s="10">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D50" s="10">
         <v>0</v>
       </c>
-      <c r="E50" t="s" s="11">
-        <v>49</v>
-      </c>
-      <c r="F50" t="s" s="11">
-        <v>22</v>
+      <c r="E50" s="10">
+        <v>0.67</v>
+      </c>
+      <c r="F50" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="51" ht="20.05" customHeight="1">
       <c r="A51" t="s" s="8">
-        <v>126</v>
-      </c>
-      <c r="B51" t="s" s="9">
-        <v>18</v>
+        <v>57</v>
+      </c>
+      <c r="B51" s="9">
+        <v>0.31</v>
       </c>
       <c r="C51" s="10">
-        <v>4.355</v>
+        <v>0</v>
       </c>
       <c r="D51" s="10">
-        <v>762</v>
-      </c>
-      <c r="E51" t="s" s="11">
-        <v>67</v>
-      </c>
-      <c r="F51" t="s" s="11">
-        <v>40</v>
+        <v>0</v>
+      </c>
+      <c r="E51" s="10">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="F51" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="52" ht="20.05" customHeight="1">
       <c r="A52" t="s" s="8">
-        <v>127</v>
-      </c>
-      <c r="B52" t="s" s="9">
-        <v>128</v>
+        <v>58</v>
+      </c>
+      <c r="B52" s="9">
+        <v>0.42</v>
       </c>
       <c r="C52" s="10">
-        <v>302</v>
+        <v>0</v>
       </c>
       <c r="D52" s="10">
-        <v>557</v>
-      </c>
-      <c r="E52" t="s" s="11">
-        <v>26</v>
-      </c>
-      <c r="F52" t="s" s="11">
-        <v>129</v>
+        <v>0</v>
+      </c>
+      <c r="E52" s="10">
+        <v>0.58</v>
+      </c>
+      <c r="F52" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="53" ht="20.05" customHeight="1">
       <c r="A53" t="s" s="8">
-        <v>130</v>
-      </c>
-      <c r="B53" t="s" s="9">
-        <v>131</v>
+        <v>59</v>
+      </c>
+      <c r="B53" s="9">
+        <v>0.17</v>
       </c>
       <c r="C53" s="10">
-        <v>950</v>
+        <v>0</v>
       </c>
       <c r="D53" s="10">
-        <v>150</v>
-      </c>
-      <c r="E53" t="s" s="11">
-        <v>132</v>
-      </c>
-      <c r="F53" t="s" s="11">
-        <v>87</v>
+        <v>0</v>
+      </c>
+      <c r="E53" s="10">
+        <v>0.83</v>
+      </c>
+      <c r="F53" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="54" ht="20.05" customHeight="1">
       <c r="A54" t="s" s="8">
-        <v>133</v>
-      </c>
-      <c r="B54" t="s" s="9">
-        <v>12</v>
+        <v>60</v>
+      </c>
+      <c r="B54" s="9">
+        <v>0.33</v>
       </c>
       <c r="C54" s="10">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="D54" s="10">
-        <v>322</v>
-      </c>
-      <c r="E54" t="s" s="11">
-        <v>97</v>
-      </c>
-      <c r="F54" t="s" s="11">
-        <v>105</v>
+        <v>0</v>
+      </c>
+      <c r="E54" s="10">
+        <v>0.67</v>
+      </c>
+      <c r="F54" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="55" ht="20.05" customHeight="1">
       <c r="A55" t="s" s="8">
-        <v>134</v>
-      </c>
-      <c r="B55" t="s" s="9">
-        <v>18</v>
+        <v>61</v>
+      </c>
+      <c r="B55" s="9">
+        <v>0</v>
       </c>
       <c r="C55" s="10">
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="D55" s="10">
-        <v>31</v>
-      </c>
-      <c r="E55" t="s" s="11">
-        <v>100</v>
-      </c>
-      <c r="F55" t="s" s="11">
-        <v>81</v>
+        <v>0</v>
+      </c>
+      <c r="E55" s="10">
+        <v>1</v>
+      </c>
+      <c r="F55" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="56" ht="20.05" customHeight="1">
       <c r="A56" t="s" s="8">
-        <v>135</v>
-      </c>
-      <c r="B56" t="s" s="9">
-        <v>22</v>
+        <v>62</v>
+      </c>
+      <c r="B56" s="9">
+        <v>0.5</v>
       </c>
       <c r="C56" s="10">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D56" s="10">
-        <v>4</v>
-      </c>
-      <c r="E56" t="s" s="11">
-        <v>136</v>
-      </c>
-      <c r="F56" t="s" s="11">
-        <v>137</v>
+        <v>0</v>
+      </c>
+      <c r="E56" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="F56" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="57" ht="20.05" customHeight="1">
       <c r="A57" t="s" s="8">
-        <v>138</v>
-      </c>
-      <c r="B57" t="s" s="9">
-        <v>96</v>
+        <v>63</v>
+      </c>
+      <c r="B57" s="9">
+        <v>0.11</v>
       </c>
       <c r="C57" s="10">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="D57" s="10">
-        <v>55</v>
-      </c>
-      <c r="E57" t="s" s="11">
-        <v>29</v>
-      </c>
-      <c r="F57" t="s" s="11">
-        <v>139</v>
+        <v>0</v>
+      </c>
+      <c r="E57" s="10">
+        <v>0.89</v>
+      </c>
+      <c r="F57" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="58" ht="20.05" customHeight="1">
       <c r="A58" t="s" s="8">
-        <v>140</v>
-      </c>
-      <c r="B58" t="s" s="9">
-        <v>43</v>
+        <v>64</v>
+      </c>
+      <c r="B58" s="9">
+        <v>0</v>
       </c>
       <c r="C58" s="10">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="D58" s="10">
-        <v>17</v>
-      </c>
-      <c r="E58" t="s" s="11">
-        <v>141</v>
-      </c>
-      <c r="F58" t="s" s="11">
-        <v>58</v>
+        <v>0</v>
+      </c>
+      <c r="E58" s="10">
+        <v>1</v>
+      </c>
+      <c r="F58" s="10">
+        <v>1</v>
       </c>
     </row>
     <row r="59" ht="20.05" customHeight="1">
       <c r="A59" t="s" s="8">
-        <v>142</v>
-      </c>
-      <c r="B59" t="s" s="9">
-        <v>22</v>
+        <v>65</v>
+      </c>
+      <c r="B59" s="9">
+        <v>0.5</v>
       </c>
       <c r="C59" s="10">
-        <v>199</v>
+        <v>0</v>
       </c>
       <c r="D59" s="10">
         <v>0</v>
       </c>
-      <c r="E59" t="s" s="11">
-        <v>49</v>
-      </c>
-      <c r="F59" t="s" s="11">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="60" ht="20.05" customHeight="1">
-      <c r="A60" t="s" s="8">
-        <v>143</v>
-      </c>
-      <c r="B60" t="s" s="9">
-        <v>96</v>
-      </c>
-      <c r="C60" s="10">
-        <v>24</v>
-      </c>
-      <c r="D60" s="10">
-        <v>63</v>
-      </c>
-      <c r="E60" t="s" s="11">
-        <v>20</v>
-      </c>
-      <c r="F60" t="s" s="11">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="61" ht="20.05" customHeight="1">
-      <c r="A61" t="s" s="8">
-        <v>144</v>
-      </c>
-      <c r="B61" t="s" s="9">
-        <v>22</v>
-      </c>
-      <c r="C61" s="10">
-        <v>0</v>
-      </c>
-      <c r="D61" s="10">
-        <v>0</v>
-      </c>
-      <c r="E61" t="s" s="11">
-        <v>49</v>
-      </c>
-      <c r="F61" t="s" s="11">
-        <v>49</v>
+      <c r="E59" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="F59" s="10">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2970,7 +2690,7 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A42" r:id="rId1" location="" tooltip="" display="net.sourceforge.ganttproject.io"/>
+    <hyperlink ref="A41" r:id="rId1" location="" tooltip="" display="net.sourceforge.ganttproject.io"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>